<commit_message>
ACTUALIZACION DE AVANCES DE LA SEMANA
</commit_message>
<xml_diff>
--- a/Hoja de Desempeño (1).xlsx
+++ b/Hoja de Desempeño (1).xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Geovani\Desktop\PROYECTOPARCIAL2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Geovani\Desktop\PROYECTOFASE2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -897,13 +897,13 @@
                 <c:formatCode>0_);[Red]\(0\)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>4.9333333333333336</c:v>
+                  <c:v>7.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.8666666666666663</c:v>
+                  <c:v>7.3333333333333339</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.5999999999999996</c:v>
+                  <c:v>7.1333333333333329</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -915,7 +915,7 @@
                 <c:formatCode>0_);[Red]\(0\)</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4.9333333333333336</c:v>
+                  <c:v>7.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -992,13 +992,13 @@
                 <c:formatCode>0_);[Red]\(0\)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>4.9333333333333336</c:v>
+                  <c:v>7.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.8666666666666663</c:v>
+                  <c:v>7.3333333333333339</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.5999999999999996</c:v>
+                  <c:v>7.1333333333333329</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1010,7 +1010,7 @@
                 <c:formatCode>0_);[Red]\(0\)</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4.8666666666666663</c:v>
+                  <c:v>7.3333333333333339</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1087,13 +1087,13 @@
                 <c:formatCode>0_);[Red]\(0\)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>4.9333333333333336</c:v>
+                  <c:v>7.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.8666666666666663</c:v>
+                  <c:v>7.3333333333333339</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.5999999999999996</c:v>
+                  <c:v>7.1333333333333329</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1105,7 +1105,7 @@
                 <c:formatCode>0_);[Red]\(0\)</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>4.5999999999999996</c:v>
+                  <c:v>7.1333333333333329</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1182,13 +1182,13 @@
                 <c:formatCode>0_);[Red]\(0\)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>4.9333333333333336</c:v>
+                  <c:v>7.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.8666666666666663</c:v>
+                  <c:v>7.3333333333333339</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.5999999999999996</c:v>
+                  <c:v>7.1333333333333329</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1277,13 +1277,13 @@
                 <c:formatCode>0_);[Red]\(0\)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>4.9333333333333336</c:v>
+                  <c:v>7.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.8666666666666663</c:v>
+                  <c:v>7.3333333333333339</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.5999999999999996</c:v>
+                  <c:v>7.1333333333333329</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1328,13 +1328,13 @@
                 <c:formatCode>0_);[Red]\(0\)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>4.9333333333333336</c:v>
+                  <c:v>7.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.8666666666666663</c:v>
+                  <c:v>7.3333333333333339</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.5999999999999996</c:v>
+                  <c:v>7.1333333333333329</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6712,13 +6712,13 @@
                 <c:formatCode>0_);[Red]\(0\)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>4.666666666666667</c:v>
+                  <c:v>7.333333333333333</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>7.333333333333333</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.333333333333333</c:v>
+                  <c:v>6.666666666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11524,13 +11524,13 @@
                 <c:formatCode>0_);[Red]\(0\)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>4.666666666666667</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.333333333333333</c:v>
+                  <c:v>6.666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.333333333333333</c:v>
+                  <c:v>6.666666666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11670,13 +11670,13 @@
                 <c:formatCode>0_);[Red]\(0\)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>7.666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.666666666666667</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>6.333333333333333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11816,13 +11816,13 @@
                 <c:formatCode>0_);[Red]\(0\)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>5.333333333333333</c:v>
+                  <c:v>8.3333333333333339</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.333333333333333</c:v>
+                  <c:v>8.3333333333333339</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.333333333333333</c:v>
+                  <c:v>8.3333333333333339</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11962,13 +11962,13 @@
                 <c:formatCode>0_);[Red]\(0\)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>5</c:v>
+                  <c:v>7.666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>7.333333333333333</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5</c:v>
+                  <c:v>7.666666666666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12091,13 +12091,13 @@
                 <c:formatCode>0_);[Red]\(0\)</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>4.9333333333333336</c:v>
+                  <c:v>7.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.8666666666666663</c:v>
+                  <c:v>7.3333333333333339</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.5999999999999996</c:v>
+                  <c:v>7.1333333333333329</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -24981,7 +24981,7 @@
   <dimension ref="A1:AG9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="W7" sqref="W7"/>
+      <selection activeCell="AL11" sqref="AL11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25170,18 +25170,18 @@
         <v>25</v>
       </c>
       <c r="B4" s="7">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" s="35">
         <v>7</v>
       </c>
       <c r="D4" s="35">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E4" s="35"/>
       <c r="F4" s="15">
         <f t="shared" ref="F4:F6" si="0">AVERAGE(B4:E4)</f>
-        <v>4.666666666666667</v>
+        <v>7.333333333333333</v>
       </c>
       <c r="G4" s="8">
         <v>7</v>
@@ -25190,12 +25190,12 @@
         <v>7</v>
       </c>
       <c r="I4" s="8">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J4" s="8"/>
       <c r="K4" s="17">
         <f>AVERAGE(G4:J4)</f>
-        <v>4.666666666666667</v>
+        <v>7</v>
       </c>
       <c r="L4" s="9">
         <v>8</v>
@@ -25204,12 +25204,12 @@
         <v>7</v>
       </c>
       <c r="N4" s="9">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O4" s="9"/>
       <c r="P4" s="13">
         <f>AVERAGE(L4:O4)</f>
-        <v>5</v>
+        <v>7.666666666666667</v>
       </c>
       <c r="Q4" s="29">
         <v>8</v>
@@ -25218,12 +25218,12 @@
         <v>8</v>
       </c>
       <c r="S4" s="29">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="T4" s="29"/>
       <c r="U4" s="30">
         <f>AVERAGE(Q4:T4)</f>
-        <v>5.333333333333333</v>
+        <v>8.3333333333333339</v>
       </c>
       <c r="V4" s="10">
         <v>8</v>
@@ -25232,36 +25232,36 @@
         <v>7</v>
       </c>
       <c r="X4" s="10">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Y4" s="10"/>
       <c r="Z4" s="19">
         <f>AVERAGE(V4:Y4)</f>
-        <v>5</v>
+        <v>7.666666666666667</v>
       </c>
       <c r="AA4" s="11">
         <f t="shared" ref="AA4:AA6" si="1">+F4</f>
-        <v>4.666666666666667</v>
+        <v>7.333333333333333</v>
       </c>
       <c r="AB4" s="34">
         <f>+K4</f>
-        <v>4.666666666666667</v>
+        <v>7</v>
       </c>
       <c r="AC4" s="34">
         <f>+P4</f>
-        <v>5</v>
+        <v>7.666666666666667</v>
       </c>
       <c r="AD4" s="34">
         <f>+U4</f>
-        <v>5.333333333333333</v>
+        <v>8.3333333333333339</v>
       </c>
       <c r="AE4" s="34">
         <f>+Z4</f>
-        <v>5</v>
+        <v>7.666666666666667</v>
       </c>
       <c r="AF4" s="21">
         <f t="shared" ref="AF4:AF7" si="2">AVERAGE(AA4:AE4)</f>
-        <v>4.9333333333333336</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="5" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -25275,12 +25275,12 @@
         <v>7</v>
       </c>
       <c r="D5" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="16">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>7.333333333333333</v>
       </c>
       <c r="G5" s="8">
         <v>7</v>
@@ -25289,12 +25289,12 @@
         <v>6</v>
       </c>
       <c r="I5" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J5" s="2"/>
       <c r="K5" s="17">
         <f t="shared" ref="K5:K6" si="3">AVERAGE(G5:J5)</f>
-        <v>4.333333333333333</v>
+        <v>6.666666666666667</v>
       </c>
       <c r="L5" s="9">
         <v>8</v>
@@ -25303,12 +25303,12 @@
         <v>6</v>
       </c>
       <c r="N5" s="3">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="O5" s="3"/>
       <c r="P5" s="13">
         <f t="shared" ref="P5:P6" si="4">AVERAGE(L5:O5)</f>
-        <v>4.666666666666667</v>
+        <v>7</v>
       </c>
       <c r="Q5" s="29">
         <v>8</v>
@@ -25317,12 +25317,12 @@
         <v>8</v>
       </c>
       <c r="S5" s="31">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="T5" s="29"/>
       <c r="U5" s="30">
         <f t="shared" ref="U5:U6" si="5">AVERAGE(Q5:T5)</f>
-        <v>5.333333333333333</v>
+        <v>8.3333333333333339</v>
       </c>
       <c r="V5" s="10">
         <v>8</v>
@@ -25331,36 +25331,36 @@
         <v>7</v>
       </c>
       <c r="X5" s="4">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="Y5" s="4"/>
       <c r="Z5" s="19">
         <f t="shared" ref="Z5:Z6" si="6">AVERAGE(V5:Y5)</f>
-        <v>5</v>
+        <v>7.333333333333333</v>
       </c>
       <c r="AA5" s="5">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>7.333333333333333</v>
       </c>
       <c r="AB5" s="34">
         <f t="shared" ref="AB5:AB6" si="7">+K5</f>
-        <v>4.333333333333333</v>
+        <v>6.666666666666667</v>
       </c>
       <c r="AC5" s="34">
         <f t="shared" ref="AC5:AC6" si="8">+P5</f>
-        <v>4.666666666666667</v>
+        <v>7</v>
       </c>
       <c r="AD5" s="34">
         <f t="shared" ref="AD5:AD6" si="9">+U5</f>
-        <v>5.333333333333333</v>
+        <v>8.3333333333333339</v>
       </c>
       <c r="AE5" s="34">
         <f t="shared" ref="AE5:AE6" si="10">+Z5</f>
-        <v>5</v>
+        <v>7.333333333333333</v>
       </c>
       <c r="AF5" s="22">
         <f t="shared" si="2"/>
-        <v>4.8666666666666663</v>
+        <v>7.3333333333333339</v>
       </c>
     </row>
     <row r="6" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
@@ -25374,12 +25374,12 @@
         <v>7</v>
       </c>
       <c r="D6" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="16">
         <f t="shared" si="0"/>
-        <v>4.333333333333333</v>
+        <v>6.666666666666667</v>
       </c>
       <c r="G6" s="8">
         <v>7</v>
@@ -25388,12 +25388,12 @@
         <v>6</v>
       </c>
       <c r="I6" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="J6" s="2"/>
       <c r="K6" s="17">
         <f t="shared" si="3"/>
-        <v>4.333333333333333</v>
+        <v>6.666666666666667</v>
       </c>
       <c r="L6" s="9">
         <v>6</v>
@@ -25402,12 +25402,12 @@
         <v>6</v>
       </c>
       <c r="N6" s="3">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="O6" s="3"/>
       <c r="P6" s="13">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>6.333333333333333</v>
       </c>
       <c r="Q6" s="29">
         <v>8</v>
@@ -25416,12 +25416,12 @@
         <v>8</v>
       </c>
       <c r="S6" s="31">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="T6" s="29"/>
       <c r="U6" s="30">
         <f t="shared" si="5"/>
-        <v>5.333333333333333</v>
+        <v>8.3333333333333339</v>
       </c>
       <c r="V6" s="10">
         <v>8</v>
@@ -25430,36 +25430,36 @@
         <v>7</v>
       </c>
       <c r="X6" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Y6" s="4"/>
       <c r="Z6" s="19">
         <f t="shared" si="6"/>
-        <v>5</v>
+        <v>7.666666666666667</v>
       </c>
       <c r="AA6" s="5">
         <f t="shared" si="1"/>
-        <v>4.333333333333333</v>
+        <v>6.666666666666667</v>
       </c>
       <c r="AB6" s="34">
         <f t="shared" si="7"/>
-        <v>4.333333333333333</v>
+        <v>6.666666666666667</v>
       </c>
       <c r="AC6" s="34">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>6.333333333333333</v>
       </c>
       <c r="AD6" s="34">
         <f t="shared" si="9"/>
-        <v>5.333333333333333</v>
+        <v>8.3333333333333339</v>
       </c>
       <c r="AE6" s="34">
         <f t="shared" si="10"/>
-        <v>5</v>
+        <v>7.666666666666667</v>
       </c>
       <c r="AF6" s="22">
         <f t="shared" si="2"/>
-        <v>4.5999999999999996</v>
+        <v>7.1333333333333329</v>
       </c>
     </row>
     <row r="7" spans="1:33" ht="21.75" thickBot="1" x14ac:dyDescent="0.4">
@@ -25493,27 +25493,27 @@
       <c r="Z7" s="26"/>
       <c r="AA7" s="36">
         <f>AVERAGE(AA4:AA6)</f>
-        <v>4.666666666666667</v>
+        <v>7.1111111111111107</v>
       </c>
       <c r="AB7" s="37">
         <f>AVERAGE(AB4:AB6)</f>
-        <v>4.4444444444444438</v>
+        <v>6.7777777777777786</v>
       </c>
       <c r="AC7" s="37">
         <f>AVERAGE(AC4:AC6)</f>
-        <v>4.5555555555555562</v>
+        <v>7</v>
       </c>
       <c r="AD7" s="37">
         <f>AVERAGE(AD4:AD6)</f>
-        <v>5.333333333333333</v>
+        <v>8.3333333333333339</v>
       </c>
       <c r="AE7" s="37">
         <f>AVERAGE(AE4:AE6)</f>
-        <v>5</v>
+        <v>7.5555555555555562</v>
       </c>
       <c r="AF7" s="33">
         <f t="shared" si="2"/>
-        <v>4.8</v>
+        <v>7.3555555555555561</v>
       </c>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.25">
@@ -26452,17 +26452,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="B1:F2"/>
+    <mergeCell ref="G1:K2"/>
+    <mergeCell ref="L1:P2"/>
+    <mergeCell ref="Q1:U2"/>
+    <mergeCell ref="V1:Z2"/>
     <mergeCell ref="AF2:AF3"/>
     <mergeCell ref="AA2:AA3"/>
     <mergeCell ref="AB2:AB3"/>
     <mergeCell ref="AC2:AC3"/>
     <mergeCell ref="AD2:AD3"/>
     <mergeCell ref="AE2:AE3"/>
-    <mergeCell ref="B1:F2"/>
-    <mergeCell ref="G1:K2"/>
-    <mergeCell ref="L1:P2"/>
-    <mergeCell ref="Q1:U2"/>
-    <mergeCell ref="V1:Z2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -27322,17 +27322,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="AB2:AB3"/>
-    <mergeCell ref="AC2:AC3"/>
-    <mergeCell ref="AD2:AD3"/>
-    <mergeCell ref="AE2:AE3"/>
-    <mergeCell ref="AF2:AF3"/>
     <mergeCell ref="AA2:AA3"/>
     <mergeCell ref="B1:F2"/>
     <mergeCell ref="G1:K2"/>
     <mergeCell ref="L1:P2"/>
     <mergeCell ref="Q1:U2"/>
     <mergeCell ref="V1:Z2"/>
+    <mergeCell ref="AB2:AB3"/>
+    <mergeCell ref="AC2:AC3"/>
+    <mergeCell ref="AD2:AD3"/>
+    <mergeCell ref="AE2:AE3"/>
+    <mergeCell ref="AF2:AF3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -28187,17 +28187,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="AB2:AB3"/>
-    <mergeCell ref="AC2:AC3"/>
-    <mergeCell ref="AD2:AD3"/>
-    <mergeCell ref="AE2:AE3"/>
-    <mergeCell ref="AF2:AF3"/>
     <mergeCell ref="AA2:AA3"/>
     <mergeCell ref="B1:F2"/>
     <mergeCell ref="G1:K2"/>
     <mergeCell ref="L1:P2"/>
     <mergeCell ref="Q1:U2"/>
     <mergeCell ref="V1:Z2"/>
+    <mergeCell ref="AB2:AB3"/>
+    <mergeCell ref="AC2:AC3"/>
+    <mergeCell ref="AD2:AD3"/>
+    <mergeCell ref="AE2:AE3"/>
+    <mergeCell ref="AF2:AF3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>